<commit_message>
feat: datamanager with cardinfo loading
</commit_message>
<xml_diff>
--- a/Assets/Resources/DataTablePrototype/ETS_datatable.xlsx
+++ b/Assets/Resources/DataTablePrototype/ETS_datatable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghj45\OneDrive\바탕 화면\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghj45\ExorciseTheSpecter\Assets\Resources\DataTablePrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B0E0BE-2A4A-438C-B8D8-243B501B2FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF5D052-F36A-4D0F-952D-24A61212A57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="5" xr2:uid="{7DC5B7CE-CBBC-406C-8CA9-789807752220}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{7DC5B7CE-CBBC-406C-8CA9-789807752220}"/>
   </bookViews>
   <sheets>
     <sheet name="StageInfo" sheetId="5" r:id="rId1"/>
@@ -1591,7 +1591,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1764,6 +1764,9 @@
       <c r="A8">
         <v>1</v>
       </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
       <c r="C8">
         <v>1</v>
       </c>
@@ -1784,6 +1787,9 @@
       <c r="A9">
         <v>1</v>
       </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
       <c r="C9">
         <v>1</v>
       </c>
@@ -1804,6 +1810,9 @@
       <c r="A10">
         <v>1</v>
       </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
       <c r="C10">
         <v>1</v>
       </c>
@@ -1824,6 +1833,9 @@
       <c r="A11">
         <v>1</v>
       </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
       <c r="C11">
         <v>1</v>
       </c>
@@ -1844,6 +1856,9 @@
       <c r="A12">
         <v>1</v>
       </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
       <c r="C12">
         <v>2</v>
       </c>
@@ -1864,6 +1879,9 @@
       <c r="A13">
         <v>1</v>
       </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
       <c r="C13">
         <v>2</v>
       </c>
@@ -1884,6 +1902,9 @@
       <c r="A14">
         <v>1</v>
       </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
       <c r="C14">
         <v>2</v>
       </c>
@@ -1904,6 +1925,9 @@
       <c r="A15">
         <v>1</v>
       </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
       <c r="C15">
         <v>2</v>
       </c>
@@ -1924,6 +1948,9 @@
       <c r="A16">
         <v>1</v>
       </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
       <c r="C16">
         <v>3</v>
       </c>
@@ -1944,6 +1971,9 @@
       <c r="A17">
         <v>1</v>
       </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
       <c r="C17">
         <v>3</v>
       </c>
@@ -1964,6 +1994,9 @@
       <c r="A18">
         <v>1</v>
       </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
       <c r="C18">
         <v>3</v>
       </c>
@@ -1984,6 +2017,9 @@
       <c r="A19">
         <v>2</v>
       </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
       <c r="C19">
         <v>1</v>
       </c>
@@ -2004,6 +2040,9 @@
       <c r="A20">
         <v>2</v>
       </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
       <c r="C20">
         <v>1</v>
       </c>
@@ -2024,6 +2063,9 @@
       <c r="A21">
         <v>2</v>
       </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
       <c r="C21">
         <v>1</v>
       </c>
@@ -2044,6 +2086,9 @@
       <c r="A22">
         <v>2</v>
       </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
       <c r="C22">
         <v>1</v>
       </c>
@@ -2064,6 +2109,9 @@
       <c r="A23">
         <v>2</v>
       </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
       <c r="C23">
         <v>2</v>
       </c>
@@ -2084,6 +2132,9 @@
       <c r="A24">
         <v>2</v>
       </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
       <c r="C24">
         <v>2</v>
       </c>
@@ -2104,6 +2155,9 @@
       <c r="A25">
         <v>2</v>
       </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
       <c r="C25">
         <v>2</v>
       </c>
@@ -2124,6 +2178,9 @@
       <c r="A26">
         <v>2</v>
       </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
       <c r="C26">
         <v>2</v>
       </c>
@@ -2144,6 +2201,9 @@
       <c r="A27">
         <v>2</v>
       </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
       <c r="C27">
         <v>3</v>
       </c>
@@ -2164,6 +2224,9 @@
       <c r="A28">
         <v>2</v>
       </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
       <c r="C28">
         <v>3</v>
       </c>
@@ -2183,6 +2246,9 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
       </c>
       <c r="C29">
         <v>3</v>

</xml_diff>

<commit_message>
docs: card info datatable modified
</commit_message>
<xml_diff>
--- a/Assets/Resources/DataTablePrototype/ETS_datatable.xlsx
+++ b/Assets/Resources/DataTablePrototype/ETS_datatable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghj45\ExorciseTheSpecter\Assets\Resources\DataTablePrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF5D052-F36A-4D0F-952D-24A61212A57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F9D2DC-5DBC-40AD-9B7A-C334EBACD5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{7DC5B7CE-CBBC-406C-8CA9-789807752220}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="173">
   <si>
     <t>스테이지번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -611,7 +611,119 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>턴 종료 시 이번 턴 동안 사용한 행동카드 당 전체마법피해2</t>
+    <t>Deal 5 physical damage.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heal 10 hp. Remove bleeding.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 5 magical damage.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Draw 2 cards.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Draw 1 card. Remove Exhausted.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 7 physical damage with 2-turn bleeding.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 4 physical damage with 2-turn bleeding.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 5 true damage.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lose 10 hp. Gain 15 extra armor.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain 5 extra armor.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 7 magical damage with 2-turn posion.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 3 magical damage to whole enemy with 2-turn dizziness.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find and bring 1 card from used card. The card costs 0.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain 1 extra composure.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 3 physical damage.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 4 physical damage. Draw 1 card.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 6 magical damage to whole enemy.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 4 damage to random target for 8 times.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal extra 1 magical damage for every physical damage.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain 5 extra strength. Fall into Paranoia.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain 10 extra armor. Take CounterAttack stance for 1 turn.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 15 magical damage. If any enemy killed, take Stealth stance for 1 turn.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gain extra 25 golds and heal 10 hp for every kill.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 1 magical damage to whole enemy after using every action card.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fall into Exhausted and Dizziness in this turn. Gain 1 extra intelligence for next turn.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fill your hand full of "Single Shot" cards. Fall into Exhausted and Dizziness in next turn.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Give every enemy 2-turn Exhausted and Paranoia.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>턴 종료 시 무작위 적에게 마법피해4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal 4 magical damage to random target every end of player's turn.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1591,10 +1703,16 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="19.875" customWidth="1"/>
+    <col min="7" max="7" width="55" customWidth="1"/>
+    <col min="8" max="8" width="75.875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1641,6 +1759,9 @@
       <c r="F2" t="s">
         <v>61</v>
       </c>
+      <c r="G2" t="s">
+        <v>144</v>
+      </c>
       <c r="H2" t="s">
         <v>67</v>
       </c>
@@ -1664,6 +1785,9 @@
       <c r="F3" t="s">
         <v>63</v>
       </c>
+      <c r="G3" t="s">
+        <v>153</v>
+      </c>
       <c r="H3" t="s">
         <v>68</v>
       </c>
@@ -1687,6 +1811,9 @@
       <c r="F4" t="s">
         <v>65</v>
       </c>
+      <c r="G4" t="s">
+        <v>145</v>
+      </c>
       <c r="H4" t="s">
         <v>69</v>
       </c>
@@ -1710,6 +1837,9 @@
       <c r="F5" t="s">
         <v>71</v>
       </c>
+      <c r="G5" t="s">
+        <v>146</v>
+      </c>
       <c r="H5" t="s">
         <v>72</v>
       </c>
@@ -1733,6 +1863,9 @@
       <c r="F6" t="s">
         <v>73</v>
       </c>
+      <c r="G6" t="s">
+        <v>147</v>
+      </c>
       <c r="H6" t="s">
         <v>75</v>
       </c>
@@ -1756,6 +1889,9 @@
       <c r="F7" t="s">
         <v>74</v>
       </c>
+      <c r="G7" t="s">
+        <v>148</v>
+      </c>
       <c r="H7" t="s">
         <v>76</v>
       </c>
@@ -1779,6 +1915,9 @@
       <c r="F8" t="s">
         <v>80</v>
       </c>
+      <c r="G8" t="s">
+        <v>149</v>
+      </c>
       <c r="H8" t="s">
         <v>107</v>
       </c>
@@ -1802,6 +1941,9 @@
       <c r="F9" t="s">
         <v>122</v>
       </c>
+      <c r="G9" t="s">
+        <v>150</v>
+      </c>
       <c r="H9" t="s">
         <v>108</v>
       </c>
@@ -1825,6 +1967,9 @@
       <c r="F10" t="s">
         <v>81</v>
       </c>
+      <c r="G10" t="s">
+        <v>151</v>
+      </c>
       <c r="H10" t="s">
         <v>82</v>
       </c>
@@ -1848,6 +1993,9 @@
       <c r="F11" t="s">
         <v>79</v>
       </c>
+      <c r="G11" t="s">
+        <v>152</v>
+      </c>
       <c r="H11" t="s">
         <v>83</v>
       </c>
@@ -1871,6 +2019,9 @@
       <c r="F12" t="s">
         <v>84</v>
       </c>
+      <c r="G12" t="s">
+        <v>154</v>
+      </c>
       <c r="H12" t="s">
         <v>88</v>
       </c>
@@ -1894,6 +2045,9 @@
       <c r="F13" t="s">
         <v>85</v>
       </c>
+      <c r="G13" t="s">
+        <v>155</v>
+      </c>
       <c r="H13" t="s">
         <v>109</v>
       </c>
@@ -1917,6 +2071,9 @@
       <c r="F14" t="s">
         <v>86</v>
       </c>
+      <c r="G14" t="s">
+        <v>156</v>
+      </c>
       <c r="H14" t="s">
         <v>89</v>
       </c>
@@ -1940,6 +2097,9 @@
       <c r="F15" t="s">
         <v>87</v>
       </c>
+      <c r="G15" t="s">
+        <v>165</v>
+      </c>
       <c r="H15" t="s">
         <v>90</v>
       </c>
@@ -1963,6 +2123,9 @@
       <c r="F16" t="s">
         <v>91</v>
       </c>
+      <c r="G16" t="s">
+        <v>157</v>
+      </c>
       <c r="H16" t="s">
         <v>93</v>
       </c>
@@ -1986,6 +2149,9 @@
       <c r="F17" t="s">
         <v>92</v>
       </c>
+      <c r="G17" t="s">
+        <v>166</v>
+      </c>
       <c r="H17" t="s">
         <v>94</v>
       </c>
@@ -2009,8 +2175,11 @@
       <c r="F18" t="s">
         <v>142</v>
       </c>
+      <c r="G18" t="s">
+        <v>172</v>
+      </c>
       <c r="H18" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -2032,6 +2201,9 @@
       <c r="F19" t="s">
         <v>95</v>
       </c>
+      <c r="G19" t="s">
+        <v>158</v>
+      </c>
       <c r="H19" t="s">
         <v>97</v>
       </c>
@@ -2055,6 +2227,9 @@
       <c r="F20" t="s">
         <v>96</v>
       </c>
+      <c r="G20" t="s">
+        <v>159</v>
+      </c>
       <c r="H20" t="s">
         <v>98</v>
       </c>
@@ -2078,6 +2253,9 @@
       <c r="F21" t="s">
         <v>99</v>
       </c>
+      <c r="G21" t="s">
+        <v>160</v>
+      </c>
       <c r="H21" t="s">
         <v>100</v>
       </c>
@@ -2101,6 +2279,9 @@
       <c r="F22" t="s">
         <v>101</v>
       </c>
+      <c r="G22" t="s">
+        <v>161</v>
+      </c>
       <c r="H22" t="s">
         <v>102</v>
       </c>
@@ -2124,6 +2305,9 @@
       <c r="F23" t="s">
         <v>103</v>
       </c>
+      <c r="G23" t="s">
+        <v>168</v>
+      </c>
       <c r="H23" t="s">
         <v>110</v>
       </c>
@@ -2147,6 +2331,9 @@
       <c r="F24" t="s">
         <v>104</v>
       </c>
+      <c r="G24" t="s">
+        <v>170</v>
+      </c>
       <c r="H24" t="s">
         <v>111</v>
       </c>
@@ -2170,6 +2357,9 @@
       <c r="F25" t="s">
         <v>105</v>
       </c>
+      <c r="G25" t="s">
+        <v>164</v>
+      </c>
       <c r="H25" t="s">
         <v>112</v>
       </c>
@@ -2193,6 +2383,9 @@
       <c r="F26" t="s">
         <v>106</v>
       </c>
+      <c r="G26" t="s">
+        <v>169</v>
+      </c>
       <c r="H26" t="s">
         <v>113</v>
       </c>
@@ -2216,6 +2409,9 @@
       <c r="F27" t="s">
         <v>114</v>
       </c>
+      <c r="G27" t="s">
+        <v>167</v>
+      </c>
       <c r="H27" t="s">
         <v>117</v>
       </c>
@@ -2239,6 +2435,9 @@
       <c r="F28" t="s">
         <v>115</v>
       </c>
+      <c r="G28" t="s">
+        <v>163</v>
+      </c>
       <c r="H28" t="s">
         <v>118</v>
       </c>
@@ -2261,6 +2460,9 @@
       </c>
       <c r="F29" t="s">
         <v>116</v>
+      </c>
+      <c r="G29" t="s">
+        <v>162</v>
       </c>
       <c r="H29" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
docs: proposal and card effects tables
</commit_message>
<xml_diff>
--- a/Assets/Resources/DataTablePrototype/ETS_datatable.xlsx
+++ b/Assets/Resources/DataTablePrototype/ETS_datatable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghj45\ExorciseTheSpecter\Assets\Resources\DataTablePrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6D3993-8507-4025-9DB7-174BE128E113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5BB016-A297-4FE2-A427-4ABB8653A58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7DC5B7CE-CBBC-406C-8CA9-789807752220}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{7DC5B7CE-CBBC-406C-8CA9-789807752220}"/>
   </bookViews>
   <sheets>
     <sheet name="StageInfo" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="188">
   <si>
     <t>스테이지번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -304,18 +304,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>물리피해5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>방어도5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>체력회복10, 출혈 제거</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Beginner's Spellbook</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -324,10 +312,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>마법피해5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>골똘한 생각</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -336,14 +320,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2장드로우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>탈진 제거, 1장드로우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Brood Over</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -364,14 +340,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>고정피해5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>견고15, 체력-10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>맹독 주입</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -388,10 +356,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>마법피해7, 중독 2턴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>버린 카드 더미에서 카드 한 장 가져오기, 해당 카드 코스트 0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -424,30 +388,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>물리피해3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물리피해4, 1장드로우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>무차별 사격</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전체물리피해6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>눈먼 난사</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>무작위 물리피해4, 8회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>총기손질</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -464,26 +412,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>물리피해7, 출혈 2턴 부여</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물리피해4, 피해망상 2턴 부여</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체마법피해3, 전체현기증 부여</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이번 턴동안 탈진, 현기증, 다음 1턴 총명1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전체피해망상과 전체탈진 2턴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>견고10, 1턴 반격</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -508,10 +440,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>강력함5, 피해망상</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>모든 물리피해에 마법피해1 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -644,10 +572,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Lose 10 hp. Gain 15 extra armor.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Gain 5 extra armor.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -745,6 +669,122 @@
   </si>
   <si>
     <t>Armor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물리피해 5를 줍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방어도 5를 얻습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마법피해 5를 줍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카드 1장을 뽑고, 탈진을 제거합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카드 2장을 뽑습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물리피해 7을 주며, 출혈 2턴을 부여합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물리피해 4를 주며, 피해망상 2턴을 부여합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고정피해 5를 줍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력을 10 회복하고, 출혈을 제거합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>견고10, 체력-5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lose 5 hp. Gain 10 extra armor.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>힘 5를 얻고, 피해망상 상태에 빠집니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마법피해 4를 주며, 중독 2턴을 부여합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체마법피해3, 전체현기증 2턴 부여</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물리피해 3를 줍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물리피해 4를 주고, 카드 1장을 뽑습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>적전체에게 물리피해 6을 줍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무작위 물리피해 4를 줍니다. 8회 반복합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>적전체에게 탈진과 피해망상을 2턴 부여합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TypeCode1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TargetType1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectType1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectAmount1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectRepeat1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TypeCode2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TargetType2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectType2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectAmount2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectRepeat2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1172,10 +1212,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1183,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1191,7 +1231,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1520,8 +1560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0331C8E1-92D4-4BFB-8746-DB8DE3F3CDFD}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1543,7 +1583,7 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="H1" t="s">
         <v>27</v>
@@ -1777,10 +1817,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03E6D54-4A6F-4169-8538-96666A6A98A8}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1788,10 +1828,11 @@
     <col min="5" max="5" width="20.5" customWidth="1"/>
     <col min="6" max="6" width="19.875" customWidth="1"/>
     <col min="7" max="7" width="55" customWidth="1"/>
-    <col min="8" max="8" width="75.875" customWidth="1"/>
+    <col min="8" max="8" width="50.25" customWidth="1"/>
+    <col min="9" max="20" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1816,8 +1857,38 @@
       <c r="H1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>178</v>
+      </c>
+      <c r="J1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L1" t="s">
+        <v>181</v>
+      </c>
+      <c r="M1" t="s">
+        <v>182</v>
+      </c>
+      <c r="N1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O1" t="s">
+        <v>184</v>
+      </c>
+      <c r="P1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>186</v>
+      </c>
+      <c r="R1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1837,13 +1908,28 @@
         <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1863,13 +1949,28 @@
         <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1889,13 +1990,43 @@
         <v>65</v>
       </c>
       <c r="G4" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="H4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1909,19 +2040,34 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1935,19 +2081,34 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G6" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1961,19 +2122,49 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G7" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1987,19 +2178,49 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="H8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2013,19 +2234,49 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F9" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="G9" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="H9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>5</v>
+      </c>
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2039,19 +2290,34 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G10" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="H10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2065,19 +2331,49 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="H11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>10</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2091,19 +2387,49 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G12" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="H12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <v>7</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2117,19 +2443,49 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="F13" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G13" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="H13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>4</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2143,19 +2499,22 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="F14" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G14" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="H14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2169,19 +2528,37 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F15" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="H15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <v>15</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2195,19 +2572,34 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="F16" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="G16" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="H16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2221,19 +2613,22 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="F17" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G17" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="H17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2247,19 +2642,34 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="F18" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="G18" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="H18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2273,19 +2683,34 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F19" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G19" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="H19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2299,19 +2724,49 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="F20" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G20" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="H20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>4</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2325,19 +2780,34 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="F21" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G21" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="H21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>6</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2351,19 +2821,34 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="G22" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="H22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>4</v>
+      </c>
+      <c r="M22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2377,19 +2862,22 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="F23" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="G23" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="H23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2</v>
       </c>
@@ -2403,19 +2891,49 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="F24" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="G24" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="H24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>3</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+      <c r="P24">
+        <v>5</v>
+      </c>
+      <c r="Q24">
+        <v>2</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2429,19 +2947,22 @@
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="F25" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="G25" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="H25" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -2455,19 +2976,22 @@
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="F26" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="G26" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="H26" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="I26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -2481,19 +3005,22 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="F27" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="G27" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="H27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -2507,19 +3034,49 @@
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="F28" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="G28" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="H28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>5</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>3</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>5</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -2533,16 +3090,19 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="F29" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="G29" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="H29" t="s">
-        <v>119</v>
+        <v>101</v>
+      </c>
+      <c r="I29">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: datamanager load card efxs
</commit_message>
<xml_diff>
--- a/Assets/Resources/DataTablePrototype/ETS_datatable.xlsx
+++ b/Assets/Resources/DataTablePrototype/ETS_datatable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghj45\ExorciseTheSpecter\Assets\Resources\DataTablePrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5BB016-A297-4FE2-A427-4ABB8653A58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FF19DE-1E19-400B-9A7D-A1BE520FE86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{7DC5B7CE-CBBC-406C-8CA9-789807752220}"/>
   </bookViews>
@@ -1820,7 +1820,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>